<commit_message>
Update for Phase 1+2 focus areas
Close to final version for Stage 1 Pollution Assessment report.
</commit_message>
<xml_diff>
--- a/data/cluster_loads.xlsx
+++ b/data/cluster_loads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaufdenkampe/Documents/Python/WikiSRATMicroService/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF89BAA8-A6D0-5645-AD77-FDB95A79E3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E5AF75-DE40-3F41-9F30-2A625143CABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15200" yWindow="-21140" windowWidth="21880" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10080" yWindow="460" windowWidth="25320" windowHeight="21640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cluster_loads" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="68">
   <si>
     <t>cluster</t>
   </si>
@@ -237,6 +237,9 @@
   <si>
     <t>or other areas</t>
   </si>
+  <si>
+    <t>Used by Barry for Cost Estimates</t>
+  </si>
 </sst>
 </file>
 
@@ -245,7 +248,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,6 +458,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9900FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -513,7 +530,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -692,6 +709,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1088,7 +1107,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
+      <selection pane="bottomRight" activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2457,13 +2476,16 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="O13" s="12">
+      <c r="O13" s="82">
         <f t="shared" si="19"/>
         <v>416267.3949433869</v>
       </c>
-      <c r="P13" s="12">
+      <c r="P13" s="82">
         <f t="shared" si="19"/>
         <v>5737168.4243200002</v>
+      </c>
+      <c r="Q13" s="83" t="s">
+        <v>67</v>
       </c>
       <c r="AB13" s="7"/>
       <c r="AC13" s="7"/>
@@ -8110,8 +8132,8 @@
   </sheetPr>
   <dimension ref="A2:AM1012"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K28" sqref="K1:L1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8334,10 +8356,10 @@
         <v>tn_load_avoid</v>
       </c>
       <c r="J5" s="36"/>
-      <c r="K5" s="82" t="s">
+      <c r="K5" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="83"/>
+      <c r="L5" s="85"/>
       <c r="M5" s="57"/>
       <c r="N5" s="57"/>
       <c r="O5" s="57"/>
@@ -9855,10 +9877,10 @@
         <v>tp_load_avoid</v>
       </c>
       <c r="J24" s="24"/>
-      <c r="K24" s="82" t="s">
+      <c r="K24" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="83"/>
+      <c r="L24" s="85"/>
       <c r="M24" s="61"/>
       <c r="N24" s="61"/>
       <c r="O24" s="61"/>
@@ -11464,10 +11486,10 @@
         <v>tss_load_avoid</v>
       </c>
       <c r="J43" s="36"/>
-      <c r="K43" s="82" t="s">
+      <c r="K43" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="L43" s="83"/>
+      <c r="L43" s="85"/>
       <c r="M43" s="57"/>
       <c r="N43" s="57"/>
       <c r="O43" s="57"/>

</xml_diff>